<commit_message>
🚀[NEW] Support vLLM.LLM ; small fixes
</commit_message>
<xml_diff>
--- a/asset/DevelopmentStatistics.xlsx
+++ b/asset/DevelopmentStatistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wumengsong/Code/Github/FastMindAPI/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE753F84-8E07-D447-9498-A1438FD39B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EE5D92-4C83-0F46-9436-F76D9E38585C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46920" yWindow="1400" windowWidth="34100" windowHeight="23300" xr2:uid="{A0AB7DDA-DAF9-6249-AD08-B2423C10C969}"/>
+    <workbookView xWindow="35960" yWindow="1760" windowWidth="45480" windowHeight="23300" xr2:uid="{A0AB7DDA-DAF9-6249-AD08-B2423C10C969}"/>
   </bookViews>
   <sheets>
     <sheet name="OptionalKwargs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="27">
   <si>
     <t>Model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -138,13 +138,17 @@
   </si>
   <si>
     <t>✍️</t>
+  </si>
+  <si>
+    <t>vLLMLLM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -165,15 +169,6 @@
       <color theme="1"/>
       <name val="等线"/>
       <family val="4"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="等线"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -284,15 +279,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -328,10 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -351,9 +340,8 @@
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -672,7 +660,7 @@
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="C1" sqref="C1:E1048576"/>
       <selection pane="bottomLeft" sqref="A1:B1"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -685,10 +673,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
@@ -698,20 +686,20 @@
       <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="15"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
@@ -724,20 +712,22 @@
       <c r="E3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="18">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="16"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
@@ -750,11 +740,13 @@
       <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="16"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -767,9 +759,12 @@
       <c r="E6" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="16"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -782,9 +777,12 @@
       <c r="E7" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="16"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -797,9 +795,12 @@
       <c r="E8" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="16"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -812,9 +813,12 @@
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="16"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -827,9 +831,12 @@
       <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="16"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
@@ -842,9 +849,12 @@
       <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="16"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="5" t="s">
         <v>13</v>
       </c>
@@ -857,9 +867,12 @@
       <c r="E12" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F12" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="15"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -872,9 +885,12 @@
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="F13" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -882,13 +898,13 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="16"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="16"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="4" t="s">
         <v>19</v>
       </c>
@@ -901,9 +917,12 @@
       <c r="E16" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="16"/>
+      <c r="F16" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="15"/>
       <c r="B17" s="4" t="s">
         <v>20</v>
       </c>
@@ -916,9 +935,12 @@
       <c r="E17" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="16"/>
+      <c r="F17" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="15"/>
       <c r="B18" s="4" t="s">
         <v>21</v>
       </c>
@@ -931,9 +953,12 @@
       <c r="E18" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="15"/>
+      <c r="F18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="14"/>
       <c r="B19" s="4" t="s">
         <v>22</v>
       </c>
@@ -944,6 +969,9 @@
         <v>23</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>